<commit_message>
mapa completo, y recoleccion de datos
</commit_message>
<xml_diff>
--- a/Data/Incendios Forestales/Incidentes.xlsx
+++ b/Data/Incendios Forestales/Incidentes.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Universidad\IA II\Paper\Data\Incendios Forestales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Universidad\IA II\Paper\paperIncendiosForestales\Data\Incendios Forestales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFED47E5-5E56-4D22-8263-359687C707A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4425ABFE-59BE-4A9A-9975-15669FFD8BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="2" r:id="rId1"/>
     <sheet name="2021" sheetId="1" r:id="rId2"/>
     <sheet name="2022" sheetId="3" r:id="rId3"/>
     <sheet name="2023" sheetId="4" r:id="rId4"/>
+    <sheet name="Consolidado" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="9">
   <si>
     <t>BOGOTA, D.C.</t>
   </si>
@@ -65,7 +66,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,8 +134,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +175,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
@@ -231,7 +251,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -332,6 +352,61 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -617,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76374FCC-5295-4D9F-8391-1AA3130395FC}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E8"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +847,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +890,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D9F769-AE99-4455-A23F-39FA1C5123B9}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,4 +1168,384 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430A6C96-D594-485E-A349-D3681741EF97}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>43839</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="34"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>43877</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>43879</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="34"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>43894</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="35"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>44046</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="34"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>44058</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>44178</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="34"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>44217</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>44590</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>44592</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>44822</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="44">
+        <v>44953</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="45">
+        <v>44959</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="44">
+        <v>45052</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="45">
+        <v>45180</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="44">
+        <v>45199</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="45">
+        <v>45202</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="44">
+        <v>45208</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="45">
+        <v>45218</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="44">
+        <v>45219</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="52"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="28">
+        <v>45264</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="28">
+        <v>45267</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>45273</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:D4 B5:C7" xr:uid="{7821F001-A3B6-4F03-8B0C-A49C980139B4}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>